<commit_message>
Changes to GINI P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P2.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0198A50-B3EF-43E0-B4E1-8E74E989B188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348ABFE6-2950-40A3-8DE8-12D06B9DD82E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
   <si>
     <t>index</t>
   </si>
@@ -43,18 +43,12 @@
     <t>ID of the participant</t>
   </si>
   <si>
-    <t>text</t>
+    <t>integer</t>
   </si>
   <si>
     <t xml:space="preserve">GESCHL </t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>KIALTER_15</t>
   </si>
   <si>
@@ -67,15 +61,9 @@
     <t>gsc09m</t>
   </si>
   <si>
-    <t>highest education of the mother</t>
-  </si>
-  <si>
     <t>gsc08v</t>
   </si>
   <si>
-    <t>highest education of the father</t>
-  </si>
-  <si>
     <t>mutberuztak3_15</t>
   </si>
   <si>
@@ -94,6 +82,9 @@
     <t>Nationality of Parents</t>
   </si>
   <si>
+    <t>Number of hours in a normal week (7 days) with heavy physical activity (a lot of sweating, rapid breathing, e.g. ball games, training) in summer [hours]</t>
+  </si>
+  <si>
     <t>K_FB_rauchkind_15</t>
   </si>
   <si>
@@ -106,30 +97,12 @@
     <t>Multivitamin supplements use</t>
   </si>
   <si>
-    <t xml:space="preserve">KE_menstr_15 </t>
-  </si>
-  <si>
-    <t>For girls: Statement by the participant about the onset of menstruation (period)</t>
-  </si>
-  <si>
-    <t>KE_pille_15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For girls: taking the contraceptive pill </t>
-  </si>
-  <si>
     <t xml:space="preserve">TG_15 </t>
   </si>
   <si>
-    <t>triglycerides</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHOL_15 </t>
   </si>
   <si>
-    <t>cholesterol</t>
-  </si>
-  <si>
     <t xml:space="preserve">LDLC_15 </t>
   </si>
   <si>
@@ -151,21 +124,6 @@
     <t>maligjeadalt_15</t>
   </si>
   <si>
-    <t xml:space="preserve"> Age when the malignant disease (cancer) was diagnosed by the doctor </t>
-  </si>
-  <si>
-    <t>bluthochmut_15</t>
-  </si>
-  <si>
-    <t>Doctor diagnosed high blood pressure in the birth mother</t>
-  </si>
-  <si>
-    <t>bluthochvat_15</t>
-  </si>
-  <si>
-    <t>Doctor's diagnosis of high blood pressure in the biological father</t>
-  </si>
-  <si>
     <t>diabmut_15</t>
   </si>
   <si>
@@ -181,13 +139,13 @@
     <t>KIALTER_20</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Age at 20 year follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">UB_bmi_15 </t>
   </si>
   <si>
-    <t>measured BMI</t>
+    <t>KIbmi_20</t>
   </si>
   <si>
     <t xml:space="preserve">UB_khszscore_15 </t>
@@ -196,68 +154,42 @@
     <t>BMI z-score according to Kromeyer-Hausschild in a 15-year examination</t>
   </si>
   <si>
-    <t>KIbmikhz_15</t>
-  </si>
-  <si>
     <t>UB_fmi_15</t>
   </si>
   <si>
+    <t>Calculated from BIA measurement at age 15</t>
+  </si>
+  <si>
+    <t>UB_fbm_15</t>
+  </si>
+  <si>
+    <t>Body fat mass measured by BIA</t>
+  </si>
+  <si>
     <t>FFQGCAL_15</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy intake (kilocalories) (kcal/day)
-</t>
-  </si>
-  <si>
     <t>FFQZK_15</t>
   </si>
   <si>
-    <t xml:space="preserve">absorbable Carbohydrates  intake (mg/day)
-</t>
-  </si>
-  <si>
     <t>FFQZE_15</t>
   </si>
   <si>
-    <t xml:space="preserve">Protein intake (mg/day)
-</t>
-  </si>
-  <si>
     <t>FFQZF_15</t>
   </si>
   <si>
-    <t xml:space="preserve">Fat intake (mg/day)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQZA_15 </t>
   </si>
   <si>
-    <t xml:space="preserve">Alcohol intake(Ethanol) (mg/day)
-</t>
-  </si>
-  <si>
     <t>FFQZB_15</t>
   </si>
   <si>
-    <t xml:space="preserve">Fiber intake (mg/day)
-</t>
-  </si>
-  <si>
     <t>FFQFS_15</t>
   </si>
   <si>
-    <t xml:space="preserve">saturated fat intake(mg/day)
-</t>
-  </si>
-  <si>
     <t>FFQFU_15</t>
   </si>
   <si>
-    <t xml:space="preserve">monounsaturated fat intake(mg/day)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQFP_15 </t>
   </si>
   <si>
@@ -279,15 +211,9 @@
     <t>FFQ_GI_15</t>
   </si>
   <si>
-    <t>glycaemic index</t>
-  </si>
-  <si>
     <t>FFQ_GL_15</t>
   </si>
   <si>
-    <t>glycaemic load</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQMNA_15 </t>
   </si>
   <si>
@@ -303,40 +229,25 @@
     <t>FFQSCHOKOL_15</t>
   </si>
   <si>
-    <t>chocolate in g/d</t>
-  </si>
-  <si>
     <t>FFQSCHOKOR_15</t>
   </si>
   <si>
-    <t>chocolate bars in g/d</t>
-  </si>
-  <si>
     <t>FFQGUMMIB_15</t>
   </si>
   <si>
-    <t>gummy bears in g/d</t>
-  </si>
-  <si>
     <t>FFQZUCK_15</t>
   </si>
   <si>
-    <t>sugar beet syrup in g/d</t>
-  </si>
-  <si>
     <t>FFQEIS_15</t>
   </si>
   <si>
-    <t>ice cream in g/d</t>
-  </si>
-  <si>
-    <t>biscuits in g/d</t>
-  </si>
-  <si>
-    <t>fruit cake in g/d</t>
-  </si>
-  <si>
-    <t>cream cake in g/d</t>
+    <t>FFQKEKS_15</t>
+  </si>
+  <si>
+    <t>FFQOBSTK_15</t>
+  </si>
+  <si>
+    <t>FFQTORTE_15</t>
   </si>
   <si>
     <t>FFQGEBAE_15</t>
@@ -345,7 +256,7 @@
     <t>Pastry in g/d</t>
   </si>
   <si>
-    <t>sponge cake in g/d</t>
+    <t>FFQRUEHRK_15</t>
   </si>
   <si>
     <t>FFQNEKT_15</t>
@@ -357,33 +268,18 @@
     <t>FFQFRSAFT_15</t>
   </si>
   <si>
-    <t>fruit juices in g/d</t>
-  </si>
-  <si>
     <t>FFQGESAFT_15</t>
   </si>
   <si>
-    <t>vegetable juices in g/d</t>
-  </si>
-  <si>
     <t>FFQSCHOR_15</t>
   </si>
   <si>
-    <t>diluted juices, spritzers in g/d</t>
-  </si>
-  <si>
     <t>FFQENERG_15</t>
   </si>
   <si>
-    <t>sports, energy drinks in g/d</t>
-  </si>
-  <si>
     <t>FFQCOLA_15</t>
   </si>
   <si>
-    <t>lemonade, cola, iced tea in g/d</t>
-  </si>
-  <si>
     <t>FFQSALAT_15</t>
   </si>
   <si>
@@ -432,9 +328,6 @@
     <t>Tropical fruits in g/d</t>
   </si>
   <si>
-    <t>FFQSGRUREDMEAT_15</t>
-  </si>
-  <si>
     <t>FFQAUFSCH_15</t>
   </si>
   <si>
@@ -462,9 +355,6 @@
     <t>FFQTEE_15</t>
   </si>
   <si>
-    <t>tea intake in g/d</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -549,19 +439,157 @@
     <t>don't know</t>
   </si>
   <si>
-    <t>FFQKEKS_15</t>
-  </si>
-  <si>
-    <t>FFQOBSTK_15</t>
-  </si>
-  <si>
-    <t>FFQTORTE_15</t>
-  </si>
-  <si>
-    <t>FFQRUEHRK_15</t>
-  </si>
-  <si>
-    <t>col_id</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>aktivschwintn_15</t>
+  </si>
+  <si>
+    <t>aktivleiisommn_15</t>
+  </si>
+  <si>
+    <t>aktivleiwintn_15</t>
+  </si>
+  <si>
+    <t>aktivmitsommn_15</t>
+  </si>
+  <si>
+    <t>aktivmitwintn_15</t>
+  </si>
+  <si>
+    <t>aktivschsommn_15</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Highest education of the mother</t>
+  </si>
+  <si>
+    <t>Highest education of the father</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with light physical activity of the child (without sweating, normal breathing, e.g. walking) in winter [hours]</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with moderate physical activity (a little sweating, slightly increased breathing e.g. cycling, swimming, skating) in summer [hours]</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with moderate physical activity (some sweating, slightly increased breathing e.g. cycling, swimming, skating) in winter [hours]</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with heavy physical activity (a lot of sweating, rapid breathing, e.g. ball games, training) in winter [hours]</t>
+  </si>
+  <si>
+    <t>Triglycerides</t>
+  </si>
+  <si>
+    <t>Cholesterol</t>
+  </si>
+  <si>
+    <t>Measured BMI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-reported BMI available </t>
+  </si>
+  <si>
+    <t>Absorbable Carbohydrates  intake (mg/day)</t>
+  </si>
+  <si>
+    <t>Protein intake (mg/day)</t>
+  </si>
+  <si>
+    <t>Energy intake (kilocalories) (kcal/day)</t>
+  </si>
+  <si>
+    <t>Alcohol intake(Ethanol) (mg/day)</t>
+  </si>
+  <si>
+    <t>Fat intake (mg/day)</t>
+  </si>
+  <si>
+    <t>Fiber intake (mg/day)</t>
+  </si>
+  <si>
+    <t>Saturated fat intake(mg/day)</t>
+  </si>
+  <si>
+    <t>Monounsaturated fat intake(mg/day)</t>
+  </si>
+  <si>
+    <t>Glycaemic index</t>
+  </si>
+  <si>
+    <t>Glycaemic load</t>
+  </si>
+  <si>
+    <t>Chocolate in g/d</t>
+  </si>
+  <si>
+    <t>Chocolate bars in g/d</t>
+  </si>
+  <si>
+    <t>Gummy bears in g/d</t>
+  </si>
+  <si>
+    <t>Sugar beet syrup in g/d</t>
+  </si>
+  <si>
+    <t>Ice cream in g/d</t>
+  </si>
+  <si>
+    <t>Biscuits in g/d</t>
+  </si>
+  <si>
+    <t>Fruit cake in g/d</t>
+  </si>
+  <si>
+    <t>Cream cake in g/d</t>
+  </si>
+  <si>
+    <t>Sponge cake in g/d</t>
+  </si>
+  <si>
+    <t>Fruit juices in g/d</t>
+  </si>
+  <si>
+    <t>Vegetable juices in g/d</t>
+  </si>
+  <si>
+    <t>Diluted juices, spritzers in g/d</t>
+  </si>
+  <si>
+    <t>Sports, energy drinks in g/d</t>
+  </si>
+  <si>
+    <t>Lemonade, cola, iced tea in g/d</t>
+  </si>
+  <si>
+    <t>Tea intake in g/d</t>
+  </si>
+  <si>
+    <t>Number of hours in a normal week (7 days) with light physical activity of the child (without sweating, normal breathing, e.g. walking) in summer [hours]</t>
+  </si>
+  <si>
+    <t>Age when the malignant disease (cancer) was diagnosed by the doctor</t>
+  </si>
+  <si>
+    <t>FFQNUSS_15</t>
+  </si>
+  <si>
+    <t>Nuts in g/d</t>
+  </si>
+  <si>
+    <t>FFQRIND_15</t>
+  </si>
+  <si>
+    <t>Beef, veal in g/d</t>
+  </si>
+  <si>
+    <t>FFQSCHW_15</t>
+  </si>
+  <si>
+    <t>Pork in g/d</t>
   </si>
 </sst>
 </file>
@@ -611,11 +639,11 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -638,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,9 +716,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -701,18 +726,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,7 +748,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1024,20 +1044,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="4"/>
+    <col min="2" max="2" width="24.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="155.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,21 +1071,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1073,1259 +1093,1318 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6">
         <v>5</v>
       </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>24</v>
+      <c r="B11" s="24" t="s">
+        <v>140</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>28</v>
+      <c r="B13" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+        <v>149</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>35</v>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>37</v>
+      <c r="B17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>39</v>
+      <c r="B18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>40</v>
+      <c r="B19" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>43</v>
+      <c r="B20" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>45</v>
+      <c r="B21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>46</v>
+      <c r="B22" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
+      <c r="B23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>51</v>
+      <c r="B24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>53</v>
+      <c r="B25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>58</v>
+      <c r="B29" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>79</v>
+        <v>53</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>81</v>
+      <c r="B40" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>82</v>
+      <c r="B41" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>87</v>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>89</v>
+      <c r="B44" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>91</v>
+      <c r="B45" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>93</v>
+      <c r="B46" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>172</v>
+        <v>69</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>103</v>
+        <v>171</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-    </row>
-    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>116</v>
+      <c r="B60" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>118</v>
+      <c r="B61" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>120</v>
+      <c r="B62" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G62" s="5"/>
-      <c r="H62" s="15"/>
+      <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G63" s="5"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G64" s="5"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G65" s="5"/>
-      <c r="H65" s="4"/>
+      <c r="H65" s="15"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="4"/>
-      <c r="G66" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G66" s="5"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G67" s="5"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="10">
         <v>67</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>51</v>
+      <c r="B68" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G68" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G68" s="5"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>133</v>
+      <c r="B69" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>135</v>
+      <c r="B70" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G81" s="5"/>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
+        <v>74</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G83" s="4"/>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="5"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-    </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G99" s="4"/>
-    </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B112"/>
-    </row>
-    <row r="115" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
-      <c r="I115" s="4"/>
-    </row>
-    <row r="117" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G117" s="15"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G101" s="4"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
     </row>
-    <row r="118" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G118" s="15"/>
-      <c r="H118" s="4"/>
-      <c r="I118" s="4"/>
-    </row>
-    <row r="119" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G119" s="5"/>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G119" s="15"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
     </row>
-    <row r="120" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G120" s="4"/>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G120" s="15"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G121" s="4"/>
-      <c r="H121" s="7"/>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G121" s="5"/>
+      <c r="H121" s="4"/>
       <c r="I121" s="4"/>
     </row>
-    <row r="122" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G122" s="5"/>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
     </row>
-    <row r="123" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D123"/>
-    </row>
-    <row r="124" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D124"/>
-    </row>
-    <row r="125" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G123" s="4"/>
+      <c r="H123" s="7"/>
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G124" s="5"/>
+      <c r="H124" s="4"/>
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D125"/>
     </row>
-    <row r="126" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D126"/>
     </row>
-    <row r="127" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D127"/>
     </row>
-    <row r="128" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D128"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139"/>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140"/>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2335,658 +2414,504 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="14">
         <v>4</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="14">
         <v>5</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="14">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" s="14">
         <v>1</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="14">
         <v>2</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="14">
         <v>3</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="14">
         <v>4</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="14">
         <v>5</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="14">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B16" s="14">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="14">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" s="14">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="14">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B21" s="14">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B23" s="14">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="14">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B25" s="14">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26" s="14">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" s="14">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="21">
+        <v>19</v>
+      </c>
+      <c r="B28" s="20">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="21">
+        <v>19</v>
+      </c>
+      <c r="B29" s="20">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="21">
+        <v>19</v>
+      </c>
+      <c r="B30" s="20">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="21">
+        <v>19</v>
+      </c>
+      <c r="B31" s="20">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="21">
+        <v>19</v>
+      </c>
+      <c r="B32" s="20">
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="21">
+        <v>21</v>
+      </c>
+      <c r="B33" s="20">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="21">
+        <v>21</v>
+      </c>
+      <c r="B34" s="20">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="21">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="20">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="21">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="20">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="21">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="20">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="21">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="20">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="21">
-        <v>0</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="20">
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="21">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="20">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="20">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="20">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="21">
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="20">
         <v>2</v>
       </c>
-      <c r="C41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="21">
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="20">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="21">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="21">
-        <v>1</v>
-      </c>
       <c r="C44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="21">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="21">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="21">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="21">
-        <v>2</v>
-      </c>
-      <c r="C48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="21">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="21">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="21">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="21">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="21">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B54" s="21">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55" s="21">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="21">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" s="21">
-        <v>2</v>
-      </c>
-      <c r="C57" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B58" s="21">
-        <v>3</v>
-      </c>
-      <c r="C58" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2995,6 +2920,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3235,42 +3181,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A4E9A4-FD54-447B-9A2D-8F3CCEE475A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3287,9 +3201,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916FD215-94E3-49D7-AFA2-532F4DA2AAAC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
label change for FMI (GINI)
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P2.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174021BE-0AF2-43B1-8D2F-9F7B55AFB06F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F4DCCE-7CAD-4C2C-B50E-5C87A95E190D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>UB_fmi_15</t>
   </si>
   <si>
-    <t>Calculated from BIA measurement at age 15</t>
-  </si>
-  <si>
     <t>UB_fbm_15</t>
   </si>
   <si>
@@ -590,6 +587,9 @@
   </si>
   <si>
     <t xml:space="preserve">HDL_15 </t>
+  </si>
+  <si>
+    <t>FMI [kg/ m2] calculated from BIA measurement at age 15</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1093,7 +1093,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -1122,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
@@ -1136,7 +1136,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
@@ -1189,10 +1189,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>5</v>
@@ -1203,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>5</v>
@@ -1217,10 +1217,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>5</v>
@@ -1231,10 +1231,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>5</v>
@@ -1245,7 +1245,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>18</v>
@@ -1259,10 +1259,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>5</v>
@@ -1306,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>9</v>
@@ -1321,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>9</v>
@@ -1347,7 +1347,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>27</v>
@@ -1378,7 +1378,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
@@ -1435,7 +1435,7 @@
         <v>37</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
@@ -1449,7 +1449,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>9</v>
@@ -1478,7 +1478,7 @@
         <v>41</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>9</v>
@@ -1489,10 +1489,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>43</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>9</v>
@@ -1503,10 +1503,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>9</v>
@@ -1517,10 +1517,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
@@ -1531,10 +1531,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>9</v>
@@ -1545,10 +1545,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>9</v>
@@ -1559,10 +1559,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>9</v>
@@ -1573,10 +1573,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>9</v>
@@ -1587,10 +1587,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
@@ -1601,10 +1601,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -1615,10 +1615,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -1629,10 +1629,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>56</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
@@ -1643,10 +1643,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>58</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
@@ -1657,10 +1657,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>9</v>
@@ -1671,10 +1671,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>9</v>
@@ -1685,10 +1685,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>61</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>62</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
@@ -1699,10 +1699,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>9</v>
@@ -1713,10 +1713,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>9</v>
@@ -1730,10 +1730,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>9</v>
@@ -1747,10 +1747,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>9</v>
@@ -1761,10 +1761,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>9</v>
@@ -1775,10 +1775,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>9</v>
@@ -1789,10 +1789,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>9</v>
@@ -1803,10 +1803,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
@@ -1817,10 +1817,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>9</v>
@@ -1831,10 +1831,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
@@ -1845,10 +1845,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
@@ -1860,10 +1860,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
@@ -1874,10 +1874,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -1888,10 +1888,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>9</v>
@@ -1905,10 +1905,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>9</v>
@@ -1922,10 +1922,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>9</v>
@@ -1939,10 +1939,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>9</v>
@@ -1956,10 +1956,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
@@ -1973,10 +1973,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
@@ -1990,10 +1990,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>9</v>
@@ -2007,10 +2007,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>9</v>
@@ -2024,10 +2024,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>9</v>
@@ -2041,10 +2041,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>9</v>
@@ -2058,10 +2058,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>9</v>
@@ -2076,10 +2076,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>9</v>
@@ -2093,10 +2093,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>9</v>
@@ -2110,10 +2110,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>9</v>
@@ -2127,10 +2127,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>9</v>
@@ -2144,10 +2144,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>9</v>
@@ -2161,10 +2161,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>9</v>
@@ -2175,10 +2175,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>9</v>
@@ -2192,10 +2192,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>9</v>
@@ -2206,10 +2206,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>9</v>
@@ -2428,7 +2428,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,7 +2460,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,7 +2834,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2878,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2889,7 +2889,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2911,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2929,6 +2929,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3169,18 +3181,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -3190,6 +3190,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916FD215-94E3-49D7-AFA2-532F4DA2AAAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3206,15 +3217,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated GINI DD, DPE (+DATA) to update label for LDLC_15. Updated variable name + label for FFQGI_15 and FFQGL_15.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P2.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F4DCCE-7CAD-4C2C-B50E-5C87A95E190D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD21E3E3-026B-4F0D-9D04-99753C54CA03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t xml:space="preserve">LDLC_15 </t>
   </si>
   <si>
-    <t>LDL cholesterol intake</t>
-  </si>
-  <si>
     <t>HDL cholesterol [mmol/L]</t>
   </si>
   <si>
@@ -202,12 +199,6 @@
     <t>Fructose (fruit sugar) (mg)</t>
   </si>
   <si>
-    <t>FFQ_GI_15</t>
-  </si>
-  <si>
-    <t>FFQ_GL_15</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQMNA_15 </t>
   </si>
   <si>
@@ -511,12 +502,6 @@
     <t>Monounsaturated fat intake(mg/day)</t>
   </si>
   <si>
-    <t>Glycaemic index</t>
-  </si>
-  <si>
-    <t>Glycaemic load</t>
-  </si>
-  <si>
     <t>Chocolate in g/d</t>
   </si>
   <si>
@@ -590,6 +575,21 @@
   </si>
   <si>
     <t>FMI [kg/ m2] calculated from BIA measurement at age 15</t>
+  </si>
+  <si>
+    <t>LDL cholesterol [mmol/L]</t>
+  </si>
+  <si>
+    <t>FFQGI_15</t>
+  </si>
+  <si>
+    <t>FFQGL_15</t>
+  </si>
+  <si>
+    <t>Glycemic Index calculated from FFQ data</t>
+  </si>
+  <si>
+    <t>Glycemic Load calculated from FFQ data</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -1093,7 +1093,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -1122,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>5</v>
@@ -1136,7 +1136,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
@@ -1189,10 +1189,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>5</v>
@@ -1203,10 +1203,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>5</v>
@@ -1217,10 +1217,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>5</v>
@@ -1231,10 +1231,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>5</v>
@@ -1245,7 +1245,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>18</v>
@@ -1259,10 +1259,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>5</v>
@@ -1306,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>9</v>
@@ -1321,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>9</v>
@@ -1336,7 +1336,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>9</v>
@@ -1347,10 +1347,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>9</v>
@@ -1361,10 +1361,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>28</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>29</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>5</v>
@@ -1375,10 +1375,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
@@ -1389,10 +1389,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>5</v>
@@ -1404,10 +1404,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>5</v>
@@ -1418,10 +1418,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>9</v>
@@ -1432,10 +1432,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
@@ -1446,10 +1446,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>9</v>
@@ -1460,10 +1460,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>9</v>
@@ -1475,10 +1475,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>9</v>
@@ -1489,10 +1489,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>42</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>43</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>9</v>
@@ -1503,10 +1503,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>9</v>
@@ -1517,10 +1517,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
@@ -1531,10 +1531,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>9</v>
@@ -1545,10 +1545,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>9</v>
@@ -1559,10 +1559,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>9</v>
@@ -1573,10 +1573,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>9</v>
@@ -1587,10 +1587,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
@@ -1601,10 +1601,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
@@ -1615,10 +1615,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -1629,10 +1629,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
@@ -1643,10 +1643,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
@@ -1657,10 +1657,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>9</v>
@@ -1671,10 +1671,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>59</v>
+        <v>185</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>9</v>
@@ -1685,10 +1685,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
@@ -1699,10 +1699,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>9</v>
@@ -1713,10 +1713,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>9</v>
@@ -1730,10 +1730,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>9</v>
@@ -1747,10 +1747,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>9</v>
@@ -1761,10 +1761,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>9</v>
@@ -1775,10 +1775,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>9</v>
@@ -1789,10 +1789,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>9</v>
@@ -1803,10 +1803,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
@@ -1817,10 +1817,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>9</v>
@@ -1831,10 +1831,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
@@ -1845,10 +1845,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
@@ -1860,10 +1860,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
@@ -1874,10 +1874,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -1888,10 +1888,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>9</v>
@@ -1905,10 +1905,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>9</v>
@@ -1922,10 +1922,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>9</v>
@@ -1939,10 +1939,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>9</v>
@@ -1956,10 +1956,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
@@ -1973,10 +1973,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
@@ -1990,10 +1990,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>9</v>
@@ -2007,10 +2007,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>9</v>
@@ -2024,10 +2024,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>9</v>
@@ -2041,10 +2041,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>9</v>
@@ -2058,10 +2058,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>9</v>
@@ -2076,10 +2076,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>9</v>
@@ -2093,10 +2093,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>9</v>
@@ -2110,10 +2110,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>9</v>
@@ -2127,10 +2127,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>9</v>
@@ -2144,10 +2144,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>9</v>
@@ -2161,10 +2161,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>9</v>
@@ -2175,10 +2175,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>9</v>
@@ -2192,10 +2192,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>9</v>
@@ -2206,10 +2206,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>9</v>
@@ -2428,7 +2428,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,7 +2460,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2801,117 +2801,117 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="20">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="20">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="20">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="20">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="20">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="20">
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B41" s="20">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="20">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" s="20">
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="20">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2929,18 +2929,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3181,6 +3169,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -3190,17 +3190,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916FD215-94E3-49D7-AFA2-532F4DA2AAAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3217,4 +3206,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DD_GINI_P2 small change to keep consistent with P1
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_GINI_P2.xlsx
+++ b/rmonize/data_dictionary/DD_GINI_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD21E3E3-026B-4F0D-9D04-99753C54CA03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87F842C-E164-41D5-838E-1D84B1162DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="189">
   <si>
     <t>index</t>
   </si>
@@ -590,6 +590,9 @@
   </si>
   <si>
     <t>Glycemic Load calculated from FFQ data</t>
+  </si>
+  <si>
+    <t>Hochschule/Fachhochschule/Universität</t>
   </si>
 </sst>
 </file>
@@ -748,9 +751,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -788,7 +791,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -894,7 +897,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1036,7 +1039,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1046,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -2416,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +2507,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2929,6 +2932,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3169,18 +3184,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -3190,6 +3193,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{916FD215-94E3-49D7-AFA2-532F4DA2AAAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3206,15 +3220,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>